<commit_message>
Changed resitors and green LED
</commit_message>
<xml_diff>
--- a/fabrication/bom/maskmeter.xlsx
+++ b/fabrication/bom/maskmeter.xlsx
@@ -64,7 +64,7 @@
     <t>C14663</t>
   </si>
   <si>
-    <t>YELLOW LED</t>
+    <t>GREEN LED</t>
   </si>
   <si>
     <t>D1</t>
@@ -73,7 +73,7 @@
     <t>LED_SMD:LED_0805_2012Metric_Castellated</t>
   </si>
   <si>
-    <t>C2296</t>
+    <t>C375452</t>
   </si>
   <si>
     <t>RED LED</t>
@@ -85,7 +85,7 @@
     <t>C84256</t>
   </si>
   <si>
-    <t>R75</t>
+    <t>R150</t>
   </si>
   <si>
     <t>R1,R2</t>
@@ -94,7 +94,7 @@
     <t>Resistor_SMD:R_0603_1608Metric</t>
   </si>
   <si>
-    <t>C4275</t>
+    <t>C22808</t>
   </si>
   <si>
     <t>1k</t>
@@ -137,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -149,13 +149,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +179,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -187,102 +198,161 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -294,35 +364,47 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -342,8 +424,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -362,10 +446,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -542,11 +626,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -555,34 +642,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="2200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -832,10 +919,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1126,7 +1213,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1407,166 +1494,178 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.3281" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="42.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.17188" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.35156" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="8">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" t="s" s="9">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" t="s" s="9">
         <v>8</v>
       </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" t="s" s="12">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="9">
+      <c r="D4" t="s" s="12">
         <v>12</v>
       </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="A5" t="s" s="10">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" t="s" s="11">
         <v>14</v>
       </c>
-      <c r="C5" t="s" s="9">
+      <c r="C5" t="s" s="12">
         <v>15</v>
       </c>
-      <c r="D5" t="s" s="9">
+      <c r="D5" t="s" s="12">
         <v>16</v>
       </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="A6" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" t="s" s="11">
         <v>18</v>
       </c>
-      <c r="C6" t="s" s="9">
+      <c r="C6" t="s" s="12">
         <v>19</v>
       </c>
-      <c r="D6" t="s" s="9">
+      <c r="D6" t="s" s="12">
         <v>20</v>
       </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="A7" t="s" s="10">
         <v>21</v>
       </c>
-      <c r="B7" t="s" s="8">
+      <c r="B7" t="s" s="11">
         <v>22</v>
       </c>
-      <c r="C7" t="s" s="9">
+      <c r="C7" t="s" s="12">
         <v>19</v>
       </c>
-      <c r="D7" t="s" s="9">
+      <c r="D7" t="s" s="12">
         <v>23</v>
       </c>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="A8" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="B8" t="s" s="8">
+      <c r="B8" t="s" s="11">
         <v>25</v>
       </c>
-      <c r="C8" t="s" s="9">
+      <c r="C8" t="s" s="12">
         <v>26</v>
       </c>
-      <c r="D8" t="s" s="9">
+      <c r="D8" t="s" s="12">
         <v>27</v>
       </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="7">
+      <c r="A9" t="s" s="10">
         <v>28</v>
       </c>
-      <c r="B9" t="s" s="8">
+      <c r="B9" t="s" s="11">
         <v>29</v>
       </c>
-      <c r="C9" t="s" s="9">
+      <c r="C9" t="s" s="12">
         <v>26</v>
       </c>
-      <c r="D9" t="s" s="9">
+      <c r="D9" t="s" s="12">
         <v>30</v>
       </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="7">
+      <c r="A10" t="s" s="10">
         <v>31</v>
       </c>
-      <c r="B10" t="s" s="8">
+      <c r="B10" t="s" s="11">
         <v>32</v>
       </c>
-      <c r="C10" t="s" s="9">
+      <c r="C10" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="D10" t="s" s="9">
+      <c r="D10" t="s" s="12">
         <v>34</v>
       </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="7">
+      <c r="A11" t="s" s="10">
         <v>35</v>
       </c>
-      <c r="B11" t="s" s="8">
+      <c r="B11" t="s" s="11">
         <v>36</v>
       </c>
-      <c r="C11" t="s" s="9">
+      <c r="C11" t="s" s="12">
         <v>37</v>
       </c>
-      <c r="D11" t="s" s="9">
+      <c r="D11" t="s" s="12">
         <v>38</v>
       </c>
+      <c r="E11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>